<commit_message>
more timings and plots
</commit_message>
<xml_diff>
--- a/Timings.xlsx
+++ b/Timings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\COSC6376-Cloud\project\BuildVoterDatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EBFF4B-9FB0-4C67-90B1-FF0F835D7ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7562AED4-92C4-4EFB-B112-79013FDF2CE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="-120" windowWidth="36855" windowHeight="14745" xr2:uid="{D0C4C60E-E71B-4053-B028-600BDBC10FF6}"/>
+    <workbookView xWindow="30195" yWindow="-120" windowWidth="25185" windowHeight="14685" activeTab="1" xr2:uid="{D0C4C60E-E71B-4053-B028-600BDBC10FF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="100">
   <si>
     <t>Blocksize</t>
   </si>
@@ -323,6 +323,21 @@
   </si>
   <si>
     <t>B-8192</t>
+  </si>
+  <si>
+    <t>ios2</t>
+  </si>
+  <si>
+    <t>512 logical sector 512 physical  buffered reads 330 MB/sec 100 IOPS</t>
+  </si>
+  <si>
+    <t>lscp</t>
+  </si>
+  <si>
+    <t>io2</t>
+  </si>
+  <si>
+    <t>blocksize</t>
   </si>
 </sst>
 </file>
@@ -1033,7 +1048,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1121,6 +1136,121 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="4"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1820,7 +1950,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1908,6 +2038,671 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="4"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1"/>
+              <a:t>Random</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" b="1" baseline="0"/>
+              <a:t> Access IO</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$C$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>gp2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$B$33:$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$C$33:$C$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0416799999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1939699999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9949400000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0119-4760-B3B8-616DFB008D0E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$D$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>gp3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="00B050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$B$33:$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$D$33:$D$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0434380000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1700200000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9953600000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0119-4760-B3B8-616DFB008D0E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$E$32</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>io2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$B$33:$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$E$33:$E$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.98940000000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1424799999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9087399999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0119-4760-B3B8-616DFB008D0E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="582589432"/>
+        <c:axId val="582594112"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="582589432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="582594112"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="582594112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="582589432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="0"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2022,6 +2817,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3067,6 +3902,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3077,9 +4415,9 @@
       <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3108,15 +4446,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3136,6 +4474,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>4762</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4BD97189-4C05-7F80-5590-75833079239B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3441,10 +4815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD1D8C9-CB71-4365-851C-1CECA1F9A8AB}">
-  <dimension ref="A1:AN68"/>
+  <dimension ref="A1:AN78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="L37" sqref="L1:AD1048576"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3454,7 +4828,9 @@
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
     <col min="4" max="5" width="14.5703125" customWidth="1"/>
     <col min="6" max="6" width="14.140625" customWidth="1"/>
-    <col min="10" max="34" width="9.140625" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="24" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="25" max="34" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.25">
@@ -5815,6 +7191,9 @@
       <c r="A37" t="s">
         <v>65</v>
       </c>
+      <c r="C37" t="s">
+        <v>92</v>
+      </c>
       <c r="D37" s="2" t="s">
         <v>76</v>
       </c>
@@ -6008,6 +7387,12 @@
       <c r="X40">
         <v>1.266</v>
       </c>
+      <c r="Z40">
+        <v>3.972</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>97</v>
+      </c>
       <c r="AD40">
         <v>4.5860000000000003</v>
       </c>
@@ -6806,6 +8191,9 @@
       </c>
     </row>
     <row r="53" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>90</v>
+      </c>
       <c r="B53" t="s">
         <v>87</v>
       </c>
@@ -7044,6 +8432,9 @@
       </c>
     </row>
     <row r="62" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>92</v>
+      </c>
       <c r="J62">
         <v>1.167</v>
       </c>
@@ -7293,6 +8684,284 @@
       <c r="D68">
         <f>SUM(AF62:AF66)/5</f>
         <v>1.9936399999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>65</v>
+      </c>
+      <c r="C71" t="s">
+        <v>95</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J71" t="s">
+        <v>89</v>
+      </c>
+      <c r="T71" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y71" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD71" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="72" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>95</v>
+      </c>
+      <c r="J72">
+        <v>1.0940000000000001</v>
+      </c>
+      <c r="K72">
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="L72">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="T72">
+        <v>1.325</v>
+      </c>
+      <c r="U72">
+        <v>1.1705000000000001</v>
+      </c>
+      <c r="V72">
+        <v>1.649</v>
+      </c>
+      <c r="Y72">
+        <v>1.395</v>
+      </c>
+      <c r="Z72">
+        <v>1.2609999999999999</v>
+      </c>
+      <c r="AA72">
+        <v>1.2589999999999999</v>
+      </c>
+      <c r="AD72">
+        <v>2.0590000000000002</v>
+      </c>
+      <c r="AE72">
+        <v>1.9319999999999999</v>
+      </c>
+      <c r="AF72">
+        <v>1.9339999999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>512</v>
+      </c>
+      <c r="B73">
+        <f>SUM(J72:J76)/5</f>
+        <v>1.0904800000000001</v>
+      </c>
+      <c r="C73">
+        <f>SUM(K72:K76)/5</f>
+        <v>0.98940000000000006</v>
+      </c>
+      <c r="D73">
+        <f>SUM(L72:L76)/5</f>
+        <v>0.98429999999999995</v>
+      </c>
+      <c r="J73">
+        <v>1.0820000000000001</v>
+      </c>
+      <c r="K73">
+        <v>0.98299999999999998</v>
+      </c>
+      <c r="L73">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="T73">
+        <v>1.216</v>
+      </c>
+      <c r="U73">
+        <v>1.115</v>
+      </c>
+      <c r="V73">
+        <v>1.113</v>
+      </c>
+      <c r="Y73">
+        <v>1.3204</v>
+      </c>
+      <c r="Z73">
+        <v>1.2184999999999999</v>
+      </c>
+      <c r="AA73">
+        <v>1.2190000000000001</v>
+      </c>
+      <c r="AD73">
+        <v>2.032</v>
+      </c>
+      <c r="AE73">
+        <v>1.9330000000000001</v>
+      </c>
+      <c r="AF73">
+        <v>1.9315</v>
+      </c>
+    </row>
+    <row r="74" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="J74">
+        <v>1.083</v>
+      </c>
+      <c r="K74">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="L74">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="T74">
+        <v>1.26</v>
+      </c>
+      <c r="U74">
+        <v>1.1592</v>
+      </c>
+      <c r="V74">
+        <v>1.1588000000000001</v>
+      </c>
+      <c r="Y74">
+        <v>1.3360000000000001</v>
+      </c>
+      <c r="Z74">
+        <v>1.212</v>
+      </c>
+      <c r="AA74">
+        <v>1.212</v>
+      </c>
+      <c r="AD74">
+        <v>2.0222000000000002</v>
+      </c>
+      <c r="AE74">
+        <v>1.9179999999999999</v>
+      </c>
+      <c r="AF74">
+        <v>1.9256</v>
+      </c>
+    </row>
+    <row r="75" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>4096</v>
+      </c>
+      <c r="B75">
+        <f>SUM(T72:T76)/5</f>
+        <v>1.2574999999999998</v>
+      </c>
+      <c r="C75">
+        <f>SUM(U72:U76)/5</f>
+        <v>1.1424799999999999</v>
+      </c>
+      <c r="D75">
+        <f>SUM(V72:V76)/5</f>
+        <v>1.2363</v>
+      </c>
+      <c r="J75">
+        <v>1.093</v>
+      </c>
+      <c r="K75">
+        <v>0.999</v>
+      </c>
+      <c r="L75">
+        <v>0.99850000000000005</v>
+      </c>
+      <c r="T75">
+        <v>1.2470000000000001</v>
+      </c>
+      <c r="U75">
+        <v>1.1316999999999999</v>
+      </c>
+      <c r="V75">
+        <v>1.1287</v>
+      </c>
+      <c r="Y75">
+        <v>1.349</v>
+      </c>
+      <c r="Z75">
+        <v>1.2270000000000001</v>
+      </c>
+      <c r="AA75">
+        <v>1.2298</v>
+      </c>
+      <c r="AD75">
+        <v>1.9770000000000001</v>
+      </c>
+      <c r="AE75">
+        <v>1.9036999999999999</v>
+      </c>
+      <c r="AF75">
+        <v>1.9103000000000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>8192</v>
+      </c>
+      <c r="B76">
+        <f>SUM(Y72:Y76)/5</f>
+        <v>1.34528</v>
+      </c>
+      <c r="C76">
+        <f>SUM(Z72:Z76)/5</f>
+        <v>1.2258599999999999</v>
+      </c>
+      <c r="D76">
+        <f>SUM(AA72:AA76)/5</f>
+        <v>1.2261799999999998</v>
+      </c>
+      <c r="J76">
+        <v>1.1004</v>
+      </c>
+      <c r="K76">
+        <v>0.99199999999999999</v>
+      </c>
+      <c r="L76">
+        <v>0.97899999999999998</v>
+      </c>
+      <c r="T76">
+        <v>1.2395</v>
+      </c>
+      <c r="U76">
+        <v>1.1359999999999999</v>
+      </c>
+      <c r="V76">
+        <v>1.1319999999999999</v>
+      </c>
+      <c r="Y76">
+        <v>1.3260000000000001</v>
+      </c>
+      <c r="Z76">
+        <v>1.2108000000000001</v>
+      </c>
+      <c r="AA76">
+        <v>1.2111000000000001</v>
+      </c>
+      <c r="AD76">
+        <v>1.9850000000000001</v>
+      </c>
+      <c r="AE76">
+        <v>1.857</v>
+      </c>
+      <c r="AF76">
+        <v>1.8476999999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>32768</v>
+      </c>
+      <c r="B78">
+        <f>SUM(AD72:AD76)/5</f>
+        <v>2.0150399999999999</v>
+      </c>
+      <c r="C78">
+        <f>SUM(AE72:AE76)/5</f>
+        <v>1.9087399999999999</v>
+      </c>
+      <c r="D78">
+        <f>SUM(AF72:AF76)/5</f>
+        <v>1.9098200000000003</v>
       </c>
     </row>
   </sheetData>
@@ -7303,10 +8972,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67AE49F0-CD4C-4C3F-ACBE-BAE6ED5B0868}">
-  <dimension ref="A2:R10"/>
+  <dimension ref="A2:U48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7591,6 +9260,221 @@
       </c>
       <c r="R10">
         <v>6.0894999999999992</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B33">
+        <v>512</v>
+      </c>
+      <c r="C33">
+        <v>1.0416799999999999</v>
+      </c>
+      <c r="D33">
+        <v>1.0434380000000001</v>
+      </c>
+      <c r="E33">
+        <v>0.98940000000000006</v>
+      </c>
+    </row>
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B34">
+        <v>4096</v>
+      </c>
+      <c r="C34">
+        <v>1.1939699999999998</v>
+      </c>
+      <c r="D34">
+        <v>1.1700200000000001</v>
+      </c>
+      <c r="E34">
+        <v>1.1424799999999999</v>
+      </c>
+      <c r="N34" t="s">
+        <v>90</v>
+      </c>
+      <c r="O34" t="s">
+        <v>87</v>
+      </c>
+      <c r="P34" t="s">
+        <v>86</v>
+      </c>
+      <c r="R34" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B35">
+        <v>32768</v>
+      </c>
+      <c r="C35">
+        <v>1.9949400000000002</v>
+      </c>
+      <c r="D35">
+        <v>1.9953600000000002</v>
+      </c>
+      <c r="E35">
+        <v>1.9087399999999999</v>
+      </c>
+      <c r="N35">
+        <v>512</v>
+      </c>
+      <c r="O35">
+        <v>1.1550999999999998</v>
+      </c>
+      <c r="P35">
+        <v>1.0416799999999999</v>
+      </c>
+      <c r="R35">
+        <v>512</v>
+      </c>
+      <c r="S35">
+        <v>1.13896</v>
+      </c>
+      <c r="T35">
+        <v>1.0434380000000001</v>
+      </c>
+      <c r="U35">
+        <v>1.04226</v>
+      </c>
+    </row>
+    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="N37">
+        <v>4096</v>
+      </c>
+      <c r="O37">
+        <v>1.3118700000000001</v>
+      </c>
+      <c r="P37">
+        <v>1.1939699999999998</v>
+      </c>
+      <c r="R37">
+        <v>4096</v>
+      </c>
+      <c r="S37">
+        <v>1.27834</v>
+      </c>
+      <c r="T37">
+        <v>1.1700200000000001</v>
+      </c>
+      <c r="U37">
+        <v>1.1673999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R38">
+        <v>8192</v>
+      </c>
+      <c r="S38">
+        <v>1.4133799999999999</v>
+      </c>
+      <c r="T38">
+        <v>1.3008200000000001</v>
+      </c>
+      <c r="U38">
+        <v>1.3018000000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="N40">
+        <v>32768</v>
+      </c>
+      <c r="O40">
+        <v>2.11374</v>
+      </c>
+      <c r="P40">
+        <v>1.9949400000000002</v>
+      </c>
+      <c r="R40">
+        <v>32768</v>
+      </c>
+      <c r="S40">
+        <v>2.1332800000000001</v>
+      </c>
+      <c r="T40">
+        <v>1.9953600000000002</v>
+      </c>
+      <c r="U40">
+        <v>1.9936399999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R42" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R43">
+        <v>512</v>
+      </c>
+      <c r="S43">
+        <v>1.0904800000000001</v>
+      </c>
+      <c r="T43">
+        <v>0.98940000000000006</v>
+      </c>
+      <c r="U43">
+        <v>0.98429999999999995</v>
+      </c>
+    </row>
+    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R45">
+        <v>4096</v>
+      </c>
+      <c r="S45">
+        <v>1.2574999999999998</v>
+      </c>
+      <c r="T45">
+        <v>1.1424799999999999</v>
+      </c>
+      <c r="U45">
+        <v>1.2363</v>
+      </c>
+    </row>
+    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R46">
+        <v>8192</v>
+      </c>
+      <c r="S46">
+        <v>1.34528</v>
+      </c>
+      <c r="T46">
+        <v>1.2258599999999999</v>
+      </c>
+      <c r="U46">
+        <v>1.2261799999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="R48">
+        <v>32768</v>
+      </c>
+      <c r="S48">
+        <v>2.0150399999999999</v>
+      </c>
+      <c r="T48">
+        <v>1.9087399999999999</v>
+      </c>
+      <c r="U48">
+        <v>1.9098200000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more timings, more plots
</commit_message>
<xml_diff>
--- a/Timings.xlsx
+++ b/Timings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\COSC6376-Cloud\project\BuildVoterDatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E09BA9-7EB2-4CC9-BB79-AB64A64406B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225DFF66-0D80-460B-826E-0A068E512BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2265" yWindow="-225" windowWidth="44640" windowHeight="14685" xr2:uid="{D0C4C60E-E71B-4053-B028-600BDBC10FF6}"/>
+    <workbookView xWindow="4230" yWindow="-180" windowWidth="30345" windowHeight="15345" activeTab="1" xr2:uid="{D0C4C60E-E71B-4053-B028-600BDBC10FF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="113">
   <si>
     <t>Blocksize</t>
   </si>
@@ -354,14 +354,39 @@
   <si>
     <t>t3 large</t>
   </si>
+  <si>
+    <t>i4ixlarge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">512 logical sector 512 physical  (512 optimal) buffered reads 1050 MB/sec </t>
+  </si>
+  <si>
+    <t>fetch nokey</t>
+  </si>
+  <si>
+    <t>b2048</t>
+  </si>
+  <si>
+    <t>i4 xlarge</t>
+  </si>
+  <si>
+    <t>t3 io2</t>
+  </si>
+  <si>
+    <t>i4 (nitro)</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -412,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -420,6 +445,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1063,7 +1089,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1106,7 +1132,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1122,7 +1148,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -2008,7 +2034,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2024,7 +2050,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3403,6 +3429,1004 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Time to Build Dictionary</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$N$64</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>t2 micro</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$M$65:$M$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32678</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$N$65:$N$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.5617999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.4916</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.1882000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C7AC-44C9-8901-026950E42FC8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$O$64</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>t3 large</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$M$65:$M$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32678</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$O$65:$O$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.5595400000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.5784000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5249999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C7AC-44C9-8901-026950E42FC8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$P$64</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>d3 xlarge</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$M$65:$M$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32678</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$P$65:$P$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.1179600000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1031999999999993</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0879199999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C7AC-44C9-8901-026950E42FC8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$Q$64</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>i4 xlarge</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$M$65:$M$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32678</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$Q$65:$Q$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.27128</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2439799999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.25298</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-C7AC-44C9-8901-026950E42FC8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="620035448"/>
+        <c:axId val="620034728"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="620035448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="620034728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="620034728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="620035448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="tx1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="tx1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Random IO while reading keys</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$B$60</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>t3 io2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$A$61:$A$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$61:$B$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0904800000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2574999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0150399999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4201-4F09-9F52-6199780A3A95}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$C$60</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>D3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$A$61:$A$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$C$61:$C$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.23508</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2037200000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1371199999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4201-4F09-9F52-6199780A3A95}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$D$60</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>i4 (nitro)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet3!$A$61:$A$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>512</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4096</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$D$61:$D$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.75616000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.85816000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4287599999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4201-4F09-9F52-6199780A3A95}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:axId val="620177192"/>
+        <c:axId val="620178632"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="620177192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="620178632"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="620178632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="620177192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="tx1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -3563,6 +4587,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -5073,6 +6177,1012 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5615,16 +7725,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5687,16 +7797,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>42862</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>147637</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>347662</xdr:colOff>
-      <xdr:row>74</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>452437</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5716,6 +7826,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE3DB3EA-9359-4C64-9B8E-EEA0C4598F10}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>42862</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B8DD9C1-F4B7-D0BC-5DE6-B2C87FA104BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6021,10 +8203,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD1D8C9-CB71-4365-851C-1CECA1F9A8AB}">
-  <dimension ref="A1:AN78"/>
+  <dimension ref="A1:AY89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46:F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6034,7 +8216,12 @@
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
     <col min="4" max="5" width="14.5703125" customWidth="1"/>
     <col min="6" max="6" width="14.140625" customWidth="1"/>
-    <col min="10" max="34" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="9" width="0" hidden="1" customWidth="1"/>
+    <col min="10" max="14" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="15" max="18" width="9.140625" customWidth="1"/>
+    <col min="19" max="34" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="35" max="45" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.25">
@@ -10166,6 +12353,432 @@
       <c r="D78">
         <f>SUM(AF72:AF76)/5</f>
         <v>1.9098200000000003</v>
+      </c>
+    </row>
+    <row r="81" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>105</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="82" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>0</v>
+      </c>
+      <c r="B82" t="s">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s">
+        <v>15</v>
+      </c>
+      <c r="D82" t="s">
+        <v>2</v>
+      </c>
+      <c r="E82" t="s">
+        <v>3</v>
+      </c>
+      <c r="F82" t="s">
+        <v>47</v>
+      </c>
+      <c r="G82" t="s">
+        <v>107</v>
+      </c>
+      <c r="J82" t="s">
+        <v>75</v>
+      </c>
+      <c r="P82" t="s">
+        <v>89</v>
+      </c>
+      <c r="V82" t="s">
+        <v>108</v>
+      </c>
+      <c r="AB82" t="s">
+        <v>91</v>
+      </c>
+      <c r="AH82">
+        <v>8192</v>
+      </c>
+      <c r="AN82" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT82" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="83" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>128</v>
+      </c>
+      <c r="P83">
+        <v>3.2210000000000001</v>
+      </c>
+      <c r="Q83">
+        <v>2.972</v>
+      </c>
+      <c r="R83">
+        <v>2.7040000000000002</v>
+      </c>
+      <c r="S83">
+        <v>3.74</v>
+      </c>
+      <c r="T83">
+        <v>0.752</v>
+      </c>
+      <c r="U83">
+        <v>0.67020000000000002</v>
+      </c>
+      <c r="AB83">
+        <v>3.2223999999999999</v>
+      </c>
+      <c r="AC83">
+        <v>3.0819999999999999</v>
+      </c>
+      <c r="AD83">
+        <v>2.5339999999999998</v>
+      </c>
+      <c r="AE83">
+        <v>3.6688000000000001</v>
+      </c>
+      <c r="AF83">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="AG83">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="AT83" s="7">
+        <v>3.282</v>
+      </c>
+      <c r="AU83">
+        <v>3.0125000000000002</v>
+      </c>
+      <c r="AV83">
+        <v>2.4045000000000001</v>
+      </c>
+      <c r="AW83">
+        <v>3.5910000000000002</v>
+      </c>
+      <c r="AX83">
+        <v>1.4239999999999999</v>
+      </c>
+      <c r="AY83">
+        <v>1.3429</v>
+      </c>
+    </row>
+    <row r="84" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>512</v>
+      </c>
+      <c r="B84">
+        <f t="shared" ref="B84:G84" si="0">SUM(P83:P87)/5</f>
+        <v>3.27128</v>
+      </c>
+      <c r="C84">
+        <f t="shared" si="0"/>
+        <v>2.9648600000000003</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="0"/>
+        <v>2.7697600000000002</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="0"/>
+        <v>3.7330399999999999</v>
+      </c>
+      <c r="F84">
+        <f t="shared" si="0"/>
+        <v>0.75616000000000005</v>
+      </c>
+      <c r="G84">
+        <f t="shared" si="0"/>
+        <v>0.66701199999999994</v>
+      </c>
+      <c r="P84">
+        <v>3.2290000000000001</v>
+      </c>
+      <c r="Q84">
+        <v>2.9470000000000001</v>
+      </c>
+      <c r="R84">
+        <v>2.7519999999999998</v>
+      </c>
+      <c r="S84">
+        <v>3.6795</v>
+      </c>
+      <c r="T84">
+        <v>0.752</v>
+      </c>
+      <c r="U84">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="AB84">
+        <v>3.2726999999999999</v>
+      </c>
+      <c r="AC84">
+        <v>3.0550000000000002</v>
+      </c>
+      <c r="AD84">
+        <v>2.5346000000000002</v>
+      </c>
+      <c r="AE84">
+        <v>3.633</v>
+      </c>
+      <c r="AF84">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="AG84">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="AT84" s="7">
+        <v>3.2124999999999999</v>
+      </c>
+      <c r="AU84">
+        <v>3.0409999999999999</v>
+      </c>
+      <c r="AV84">
+        <v>2.4550000000000001</v>
+      </c>
+      <c r="AW84">
+        <v>3.6215000000000002</v>
+      </c>
+      <c r="AX84">
+        <v>1.4602999999999999</v>
+      </c>
+      <c r="AY84">
+        <v>1.353</v>
+      </c>
+    </row>
+    <row r="85" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="P85">
+        <v>3.415</v>
+      </c>
+      <c r="Q85">
+        <v>3.0013000000000001</v>
+      </c>
+      <c r="R85">
+        <v>2.9670000000000001</v>
+      </c>
+      <c r="S85">
+        <v>3.7959999999999998</v>
+      </c>
+      <c r="T85">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="U85">
+        <v>0.67959999999999998</v>
+      </c>
+      <c r="AB85">
+        <v>3.2639999999999998</v>
+      </c>
+      <c r="AC85">
+        <v>3.0139999999999998</v>
+      </c>
+      <c r="AD85">
+        <v>2.5013999999999998</v>
+      </c>
+      <c r="AE85">
+        <v>3.7124999999999999</v>
+      </c>
+      <c r="AF85">
+        <v>0.85760000000000003</v>
+      </c>
+      <c r="AG85">
+        <v>0.76949999999999996</v>
+      </c>
+      <c r="AT85" s="7">
+        <v>3.3037000000000001</v>
+      </c>
+      <c r="AU85">
+        <v>3.0527000000000002</v>
+      </c>
+      <c r="AV85">
+        <v>2.3860000000000001</v>
+      </c>
+      <c r="AW85">
+        <v>3.6697000000000002</v>
+      </c>
+      <c r="AX85">
+        <v>1.3975</v>
+      </c>
+      <c r="AY85">
+        <v>1.319</v>
+      </c>
+    </row>
+    <row r="86" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>4096</v>
+      </c>
+      <c r="B86">
+        <f t="shared" ref="B86:G86" si="1">SUM(AB83:AB87)/5</f>
+        <v>3.2439799999999996</v>
+      </c>
+      <c r="C86">
+        <f t="shared" si="1"/>
+        <v>3.0391199999999996</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="1"/>
+        <v>2.5150399999999999</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="1"/>
+        <v>3.66608</v>
+      </c>
+      <c r="F86">
+        <f t="shared" si="1"/>
+        <v>0.85816000000000003</v>
+      </c>
+      <c r="G86">
+        <f t="shared" si="1"/>
+        <v>0.76382000000000005</v>
+      </c>
+      <c r="P86">
+        <v>3.2435999999999998</v>
+      </c>
+      <c r="Q86">
+        <v>2.9620000000000002</v>
+      </c>
+      <c r="R86">
+        <v>2.6998000000000002</v>
+      </c>
+      <c r="S86">
+        <v>3.6640000000000001</v>
+      </c>
+      <c r="T86">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="U86">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="AB86">
+        <v>3.2250000000000001</v>
+      </c>
+      <c r="AC86">
+        <v>3.0070000000000001</v>
+      </c>
+      <c r="AD86">
+        <v>2.5005000000000002</v>
+      </c>
+      <c r="AE86">
+        <v>3.6093999999999999</v>
+      </c>
+      <c r="AF86">
+        <v>0.86939999999999995</v>
+      </c>
+      <c r="AG86">
+        <v>0.76800000000000002</v>
+      </c>
+      <c r="AT86" s="7">
+        <v>3.2286999999999999</v>
+      </c>
+      <c r="AU86">
+        <v>3.0186000000000002</v>
+      </c>
+      <c r="AV86">
+        <v>2.3946000000000001</v>
+      </c>
+      <c r="AW86">
+        <v>3.5844</v>
+      </c>
+      <c r="AX86">
+        <v>1.4350000000000001</v>
+      </c>
+      <c r="AY86">
+        <v>1.3286</v>
+      </c>
+    </row>
+    <row r="87" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>8192</v>
+      </c>
+      <c r="P87">
+        <v>3.2477999999999998</v>
+      </c>
+      <c r="Q87">
+        <v>2.9420000000000002</v>
+      </c>
+      <c r="R87">
+        <v>2.726</v>
+      </c>
+      <c r="S87">
+        <v>3.7856999999999998</v>
+      </c>
+      <c r="T87">
+        <v>0.74380000000000002</v>
+      </c>
+      <c r="U87">
+        <v>0.64525999999999994</v>
+      </c>
+      <c r="AB87">
+        <v>3.2357999999999998</v>
+      </c>
+      <c r="AC87">
+        <v>3.0375999999999999</v>
+      </c>
+      <c r="AD87">
+        <v>2.5047000000000001</v>
+      </c>
+      <c r="AE87">
+        <v>3.7067000000000001</v>
+      </c>
+      <c r="AF87">
+        <v>0.85780000000000001</v>
+      </c>
+      <c r="AG87">
+        <v>0.75860000000000005</v>
+      </c>
+      <c r="AT87" s="7">
+        <v>3.238</v>
+      </c>
+      <c r="AU87">
+        <v>3.0179999999999998</v>
+      </c>
+      <c r="AV87">
+        <v>2.4036</v>
+      </c>
+      <c r="AW87">
+        <v>3.6669999999999998</v>
+      </c>
+      <c r="AX87">
+        <v>1.427</v>
+      </c>
+      <c r="AY87">
+        <v>1.359</v>
+      </c>
+    </row>
+    <row r="88" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="89" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>32768</v>
+      </c>
+      <c r="B89">
+        <f>SUM(AT83:AT87)/5</f>
+        <v>3.25298</v>
+      </c>
+      <c r="C89">
+        <f>SUM(AU83:AU87)/5</f>
+        <v>3.0285600000000001</v>
+      </c>
+      <c r="D89">
+        <f>SUM(AV83:AV87)/5</f>
+        <v>2.4087400000000003</v>
+      </c>
+      <c r="E89">
+        <f>SUM(AW83:AW87)/5</f>
+        <v>3.6267200000000002</v>
+      </c>
+      <c r="F89">
+        <f>SUM(AX83:AX87)/5</f>
+        <v>1.4287599999999998</v>
+      </c>
+      <c r="G89">
+        <f>SUM(AY83:AY87)/5</f>
+        <v>1.3405</v>
       </c>
     </row>
   </sheetData>
@@ -10178,8 +12791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67AE49F0-CD4C-4C3F-ACBE-BAE6ED5B0868}">
   <dimension ref="A2:Z67"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="I67" sqref="I67"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="W55" sqref="W55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10681,7 +13294,7 @@
         <v>1.9098200000000003</v>
       </c>
     </row>
-    <row r="58" spans="13:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="O58" t="s">
         <v>101</v>
       </c>
@@ -10689,7 +13302,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="59" spans="13:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="N59" t="s">
         <v>0</v>
       </c>
@@ -10727,7 +13340,16 @@
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="13:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>110</v>
+      </c>
+      <c r="C60" t="s">
+        <v>112</v>
+      </c>
+      <c r="D60" t="s">
+        <v>111</v>
+      </c>
       <c r="N60">
         <v>512</v>
       </c>
@@ -10765,7 +13387,19 @@
         <v>1.3031999999999999</v>
       </c>
     </row>
-    <row r="61" spans="13:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>512</v>
+      </c>
+      <c r="B61">
+        <v>1.0904800000000001</v>
+      </c>
+      <c r="C61">
+        <v>1.23508</v>
+      </c>
+      <c r="D61">
+        <v>0.75616000000000005</v>
+      </c>
       <c r="M61" t="s">
         <v>100</v>
       </c>
@@ -10806,7 +13440,19 @@
         <v>1.0287999999999999</v>
       </c>
     </row>
-    <row r="62" spans="13:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>4096</v>
+      </c>
+      <c r="B62">
+        <v>1.2574999999999998</v>
+      </c>
+      <c r="C62">
+        <v>1.2037200000000001</v>
+      </c>
+      <c r="D62">
+        <v>0.85816000000000003</v>
+      </c>
       <c r="N62">
         <v>32678</v>
       </c>
@@ -10844,7 +13490,24 @@
         <v>2.0103999999999997</v>
       </c>
     </row>
-    <row r="64" spans="13:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>32768</v>
+      </c>
+      <c r="B63">
+        <v>2.0150399999999999</v>
+      </c>
+      <c r="C63">
+        <v>2.1371199999999999</v>
+      </c>
+      <c r="D63">
+        <v>1.4287599999999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="L64" t="s">
+        <v>1</v>
+      </c>
       <c r="N64" t="s">
         <v>100</v>
       </c>
@@ -10853,6 +13516,9 @@
       </c>
       <c r="P64" t="s">
         <v>103</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="65" spans="13:26" x14ac:dyDescent="0.25">
@@ -10868,6 +13534,9 @@
       <c r="P65">
         <v>4.1179600000000001</v>
       </c>
+      <c r="Q65">
+        <v>3.27128</v>
+      </c>
       <c r="U65">
         <v>512</v>
       </c>
@@ -10900,6 +13569,9 @@
       <c r="P66">
         <v>4.1031999999999993</v>
       </c>
+      <c r="Q66">
+        <v>3.2439799999999996</v>
+      </c>
       <c r="U66">
         <v>4096</v>
       </c>
@@ -10931,6 +13603,9 @@
       </c>
       <c r="P67">
         <v>4.0879199999999996</v>
+      </c>
+      <c r="Q67">
+        <v>3.25298</v>
       </c>
       <c r="U67">
         <v>32768</v>

</xml_diff>

<commit_message>
mongodb times, cleaned up plot
</commit_message>
<xml_diff>
--- a/Timings.xlsx
+++ b/Timings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\COSC6376-Cloud\project\BuildVoterDatabase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FACACF-AB88-4BEE-971B-B04FCAE28F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CBFE18-48C8-47DE-AEFB-567F9B65B127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12105" yWindow="2610" windowWidth="41595" windowHeight="15135" activeTab="1" xr2:uid="{D0C4C60E-E71B-4053-B028-600BDBC10FF6}"/>
+    <workbookView xWindow="34080" yWindow="-300" windowWidth="35475" windowHeight="15135" xr2:uid="{D0C4C60E-E71B-4053-B028-600BDBC10FF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="121">
   <si>
     <t>Blocksize</t>
   </si>
@@ -367,9 +367,6 @@
     <t>i4 xlarge</t>
   </si>
   <si>
-    <t>t3 io2</t>
-  </si>
-  <si>
     <t>i4 (nitro)</t>
   </si>
   <si>
@@ -398,6 +395,12 @@
   </si>
   <si>
     <t>t3 gp2</t>
+  </si>
+  <si>
+    <t>Mongo</t>
+  </si>
+  <si>
+    <t>read</t>
   </si>
 </sst>
 </file>
@@ -3509,7 +3512,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>t3 io2</c:v>
+                  <c:v>io2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3795,7 +3798,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1"/>
                 </a:solidFill>
@@ -6547,7 +6550,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -12221,10 +12224,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD1D8C9-CB71-4365-851C-1CECA1F9A8AB}">
-  <dimension ref="A1:AY89"/>
+  <dimension ref="A1:AY95"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63:B68"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="G95" sqref="G95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16390,7 +16393,7 @@
         <v>104</v>
       </c>
       <c r="B81" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D81" s="2" t="s">
         <v>105</v>
@@ -17161,6 +17164,54 @@
       <c r="G89">
         <f t="shared" si="5"/>
         <v>1.3405</v>
+      </c>
+    </row>
+    <row r="91" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>119</v>
+      </c>
+      <c r="B91" t="s">
+        <v>32</v>
+      </c>
+      <c r="C91" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="92" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="B92">
+        <v>270.64999999999998</v>
+      </c>
+      <c r="C92">
+        <v>27.25</v>
+      </c>
+    </row>
+    <row r="93" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="B93">
+        <v>272.95</v>
+      </c>
+      <c r="C93">
+        <v>27.34</v>
+      </c>
+      <c r="I93" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="B94">
+        <v>274.47000000000003</v>
+      </c>
+      <c r="C94">
+        <v>26.75</v>
+      </c>
+    </row>
+    <row r="95" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="B95">
+        <f>SUM(B92:B94)/3</f>
+        <v>272.69</v>
+      </c>
+      <c r="C95">
+        <f>SUM(C92:C94)/3</f>
+        <v>27.113333333333333</v>
       </c>
     </row>
   </sheetData>
@@ -17173,8 +17224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67AE49F0-CD4C-4C3F-ACBE-BAE6ED5B0868}">
   <dimension ref="A2:AT117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="Q118" sqref="Q118"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17193,10 +17244,10 @@
         <v>84</v>
       </c>
       <c r="AG2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AO2" t="s">
         <v>118</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:46" x14ac:dyDescent="0.25">
@@ -17260,19 +17311,19 @@
         <v>8</v>
       </c>
       <c r="W4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="X4" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y4" t="s">
         <v>113</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>114</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>115</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:46" x14ac:dyDescent="0.25">
@@ -18069,13 +18120,13 @@
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
+        <v>97</v>
+      </c>
+      <c r="C60" t="s">
+        <v>110</v>
+      </c>
+      <c r="D60" t="s">
         <v>109</v>
-      </c>
-      <c r="C60" t="s">
-        <v>111</v>
-      </c>
-      <c r="D60" t="s">
-        <v>110</v>
       </c>
       <c r="N60">
         <v>512</v>

</xml_diff>